<commit_message>
add EL_Price and modify forecast
</commit_message>
<xml_diff>
--- a/Set_and_Control.xlsx
+++ b/Set_and_Control.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\epish\PycharmProjects\endemo-endemo-v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A1D7D9-5044-4EA2-8E7A-387201599893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D548CE55-5549-42EF-B5D1-16E412D2849B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="730" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="730" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralSet" sheetId="22" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="UE-&gt;FE" sheetId="17" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="233">
   <si>
     <t>Activate</t>
   </si>
@@ -719,9 +720,6 @@
     <t>TEMP_DIFF_W</t>
   </si>
   <si>
-    <t>POP</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
@@ -755,9 +753,6 @@
     <t>BOF, DRI</t>
   </si>
   <si>
-    <t>SP_COOK</t>
-  </si>
-  <si>
     <t>MODAL_SUBSPLIT</t>
   </si>
   <si>
@@ -780,6 +775,21 @@
   </si>
   <si>
     <t>Useful energy types for calculation</t>
+  </si>
+  <si>
+    <t>OCCUPANT</t>
+  </si>
+  <si>
+    <t>interpolation is done with errors as we the pop if out of boundaries</t>
+  </si>
+  <si>
+    <t>COOK</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #Check the input sems like there is displacement and type name in user </t>
+  </si>
+  <si>
+    <t>#Chck belgium</t>
   </si>
 </sst>
 </file>
@@ -885,7 +895,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -895,18 +905,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1046,7 +1044,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1106,13 +1104,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1137,43 +1134,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp15.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp16.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="C2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp17.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="C2" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp18.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="C4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="C4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1181,43 +1178,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$10" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$11" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1225,43 +1222,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$15" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$16" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$16" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$17" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$17" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$18" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$20" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$22" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$22" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$23" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$23" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$24" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$24" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$25" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1269,43 +1266,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp40.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$25" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$26" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp41.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$26" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$27" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp42.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$27" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$28" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp43.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$28" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$29" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp44.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$29" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$30" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp45.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$30" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$31" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp46.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$31" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$32" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp47.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$32" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$34" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp48.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$34" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$35" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp49.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$35" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$33" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1313,43 +1310,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp50.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$33" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$36" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp51.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$36" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp52.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp53.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$15" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$16" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp54.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$16" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp55.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp56.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp57.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp58.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp59.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1357,43 +1354,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp60.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$10" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp61.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$11" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp62.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp63.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp64.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp65.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$2" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$D$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp66.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp67.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp68.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp69.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$7" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1401,43 +1398,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp70.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp71.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp72.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp73.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp74.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp75.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp76.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp77.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp74.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp75.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$6" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp78.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp77.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp78.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp79.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp79.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1445,30 +1442,26 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp80.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$2" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp81.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$5" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp82.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$C$4" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$2" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp83.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$2" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$3" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp84.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$3" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp85.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp86.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$D$12" lockText="1" noThreeD="1"/>
 </file>
 
@@ -1540,7 +1533,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1626,7 +1619,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1712,7 +1705,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1798,7 +1791,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1884,7 +1877,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1970,7 +1963,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2056,7 +2049,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2142,7 +2135,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2228,7 +2221,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2262,25 +2255,25 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>7620</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>464820</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:colOff>459105</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="40962" name="Check Box 2" hidden="1">
+            <xdr:cNvPr id="40963" name="Check Box 3" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s40962"/>
+                  <a14:compatExt spid="_x0000_s40963"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002A00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003A00000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2319,7 +2312,93 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Activate</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>472440</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="40964" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s40964"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004A00000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2354,19 +2433,19 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>464820</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="40963" name="Check Box 3" hidden="1">
+            <xdr:cNvPr id="40981" name="Check Box 21" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s40963"/>
+                  <a14:compatExt spid="_x0000_s40981"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003A00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5EAF87C-3D65-E13B-9415-CD8F8DE09B86}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2405,7 +2484,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2440,19 +2519,19 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>464820</xdr:colOff>
+          <xdr:colOff>476250</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="40964" name="Check Box 4" hidden="1">
+            <xdr:cNvPr id="40982" name="Check Box 22" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s40964"/>
+                  <a14:compatExt spid="_x0000_s40982"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004A00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{227C14DC-77C3-AE45-F84E-9E55E85AC308}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2491,7 +2570,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2517,28 +2596,23 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>7620</xdr:colOff>
-          <xdr:row>1</xdr:row>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>2</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>464820</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="1137285" cy="200025"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="40965" name="Check Box 5" hidden="1">
+            <xdr:cNvPr id="40983" name="Check Box 23" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s40965"/>
+                  <a14:compatExt spid="_x0000_s40983"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005A00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9517637C-BC88-4387-8F60-22336EC48562}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2577,7 +2651,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2597,34 +2671,29 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
+      <xdr:oneCellAnchor>
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>7620</xdr:colOff>
-          <xdr:row>2</xdr:row>
+          <xdr:colOff>9525</xdr:colOff>
+          <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>464820</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
-        </xdr:to>
+        <xdr:ext cx="1137285" cy="200025"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="40966" name="Check Box 6" hidden="1">
+            <xdr:cNvPr id="40984" name="Check Box 24" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s40966"/>
+                  <a14:compatExt spid="_x0000_s40984"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006A00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF0A1B07-581D-43F9-9FBC-D7FB86620118}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2663,7 +2732,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2683,34 +2752,39 @@
           </xdr:txBody>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:twoCellAnchor>
+      </xdr:oneCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>7620</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
+          <xdr:row>1</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>464820</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>777240</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="40967" name="Check Box 7" hidden="1">
+            <xdr:cNvPr id="21505" name="Check Box 1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s40967"/>
+                  <a14:compatExt spid="_x0000_s21505"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007A00000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001540000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2749,184 +2823,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t>Activate</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>7620</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>464820</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>22860</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="40968" name="Check Box 8" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s40968"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008A00000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr algn="l" rtl="0">
-                <a:defRPr sz="1000"/>
-              </a:pPr>
-              <a:r>
-                <a:rPr lang="en-DE" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                  <a:solidFill>
-                    <a:srgbClr val="000000"/>
-                  </a:solidFill>
-                  <a:latin typeface="Segoe UI"/>
-                  <a:cs typeface="Segoe UI"/>
-                </a:rPr>
-                <a:t>Activate</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>7620</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>784860</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="21505" name="Check Box 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s21505"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001540000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2961,9 +2858,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3012,7 +2909,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3047,9 +2944,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>3</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3098,7 +2995,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3133,9 +3030,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>1680</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3184,7 +3081,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3219,9 +3116,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3270,7 +3167,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3305,9 +3202,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3356,7 +3253,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3391,9 +3288,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>7</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3442,7 +3339,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3477,9 +3374,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3528,7 +3425,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3563,9 +3460,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3614,7 +3511,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3649,9 +3546,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3700,7 +3597,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3735,9 +3632,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>11</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3786,7 +3683,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3821,9 +3718,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>12</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>1680</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3872,7 +3769,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3907,9 +3804,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>13</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3958,7 +3855,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3993,9 +3890,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>14</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4044,7 +3941,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4079,9 +3976,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>15</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4130,7 +4027,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4165,9 +4062,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>16</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4216,7 +4113,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4251,9 +4148,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>17</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4302,7 +4199,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4337,9 +4234,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>18</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4388,7 +4285,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4423,9 +4320,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>19</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4474,7 +4371,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4509,9 +4406,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>20</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4560,7 +4457,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4595,9 +4492,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>21</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>1680</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4646,7 +4543,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4681,9 +4578,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>22</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4732,7 +4629,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4767,9 +4664,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>23</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4818,7 +4715,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4853,9 +4750,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>24</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4904,7 +4801,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4939,9 +4836,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>25</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>26</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4990,7 +4887,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5025,9 +4922,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>26</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>27</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5076,7 +4973,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5111,9 +5008,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>27</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>28</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5162,7 +5059,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5197,9 +5094,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>28</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>29</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5248,7 +5145,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5283,9 +5180,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>29</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>30</xdr:row>
+          <xdr:rowOff>1680</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5334,7 +5231,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5369,9 +5266,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>30</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>31</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5420,7 +5317,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5455,9 +5352,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>31</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>32</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5506,7 +5403,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5541,9 +5438,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
-          <xdr:row>33</xdr:row>
-          <xdr:rowOff>182880</xdr:rowOff>
+          <xdr:colOff>744855</xdr:colOff>
+          <xdr:row>34</xdr:row>
+          <xdr:rowOff>1681</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5592,7 +5489,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5627,9 +5524,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
+          <xdr:colOff>744855</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5678,7 +5575,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5713,9 +5610,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
+          <xdr:colOff>744855</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5764,7 +5661,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5799,9 +5696,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>754380</xdr:colOff>
+          <xdr:colOff>744855</xdr:colOff>
           <xdr:row>36</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5850,7 +5747,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5890,9 +5787,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>739140</xdr:colOff>
+          <xdr:colOff>742950</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>49530</xdr:rowOff>
+          <xdr:rowOff>53340</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5902,7 +5799,7 @@
                   <a14:compatExt spid="_x0000_s11267"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000032C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000032C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5941,7 +5838,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -5976,9 +5873,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>739140</xdr:colOff>
+          <xdr:colOff>742950</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -5988,7 +5885,7 @@
                   <a14:compatExt spid="_x0000_s11268"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000042C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000042C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6027,7 +5924,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6062,9 +5959,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>739140</xdr:colOff>
+          <xdr:colOff>742950</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6074,7 +5971,7 @@
                   <a14:compatExt spid="_x0000_s11269"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000052C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000052C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6113,7 +6010,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6148,9 +6045,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>739140</xdr:colOff>
+          <xdr:colOff>742950</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6160,7 +6057,7 @@
                   <a14:compatExt spid="_x0000_s11270"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000062C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000062C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6199,7 +6096,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6234,7 +6131,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>739140</xdr:colOff>
+          <xdr:colOff>742950</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -6246,7 +6143,7 @@
                   <a14:compatExt spid="_x0000_s11271"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000072C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000072C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6285,7 +6182,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6320,9 +6217,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>739140</xdr:colOff>
+          <xdr:colOff>742950</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>167640</xdr:rowOff>
+          <xdr:rowOff>171450</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6332,7 +6229,7 @@
                   <a14:compatExt spid="_x0000_s11272"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000082C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000082C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6371,7 +6268,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6406,9 +6303,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>739140</xdr:colOff>
+          <xdr:colOff>742950</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6418,7 +6315,7 @@
                   <a14:compatExt spid="_x0000_s11273"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000092C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000092C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6457,7 +6354,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6492,9 +6389,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>739140</xdr:colOff>
+          <xdr:colOff>742950</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6504,7 +6401,7 @@
                   <a14:compatExt spid="_x0000_s11274"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A2C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000A2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6543,7 +6440,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6578,9 +6475,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>739140</xdr:colOff>
+          <xdr:colOff>742950</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6590,7 +6487,7 @@
                   <a14:compatExt spid="_x0000_s11275"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B2C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6629,7 +6526,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6664,9 +6561,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>739140</xdr:colOff>
+          <xdr:colOff>742950</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>49530</xdr:rowOff>
+          <xdr:rowOff>53340</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6676,7 +6573,7 @@
                   <a14:compatExt spid="_x0000_s11276"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C2C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000C2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6715,7 +6612,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6750,9 +6647,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>739140</xdr:colOff>
+          <xdr:colOff>742950</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6762,7 +6659,7 @@
                   <a14:compatExt spid="_x0000_s11277"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D2C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000D2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6801,7 +6698,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6836,9 +6733,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>739140</xdr:colOff>
+          <xdr:colOff>742950</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>49530</xdr:rowOff>
+          <xdr:rowOff>53340</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6848,7 +6745,7 @@
                   <a14:compatExt spid="_x0000_s11294"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001E2C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001E2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6887,7 +6784,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -6922,9 +6819,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>739140</xdr:colOff>
+          <xdr:colOff>742950</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6934,7 +6831,7 @@
                   <a14:compatExt spid="_x0000_s11295"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001F2C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001F2C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6973,7 +6870,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7008,9 +6905,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>739140</xdr:colOff>
+          <xdr:colOff>742950</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>49530</xdr:rowOff>
+          <xdr:rowOff>53340</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7020,7 +6917,7 @@
                   <a14:compatExt spid="_x0000_s11303"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000272C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000272C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7059,7 +6956,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7094,9 +6991,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>739140</xdr:colOff>
+          <xdr:colOff>742950</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>15240</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7106,7 +7003,7 @@
                   <a14:compatExt spid="_x0000_s11305"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-0000292C0000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000292C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7145,7 +7042,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7197,7 +7094,7 @@
                   <a14:compatExt spid="_x0000_s16386"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002400000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002400000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7236,7 +7133,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7283,7 +7180,7 @@
                   <a14:compatExt spid="_x0000_s16387"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003400000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003400000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7322,7 +7219,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7369,7 +7266,7 @@
                   <a14:compatExt spid="_x0000_s16388"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004400000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004400000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7408,7 +7305,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7455,7 +7352,7 @@
                   <a14:compatExt spid="_x0000_s16389"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005400000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005400000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7494,7 +7391,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7541,7 +7438,7 @@
                   <a14:compatExt spid="_x0000_s16390"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006400000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006400000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7580,7 +7477,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7627,7 +7524,7 @@
                   <a14:compatExt spid="_x0000_s16391"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007400000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007400000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7666,7 +7563,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7713,7 +7610,7 @@
                   <a14:compatExt spid="_x0000_s16392"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000008400000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008400000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7752,7 +7649,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7843,7 +7740,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -7929,7 +7826,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8015,7 +7912,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8101,7 +7998,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8187,7 +8084,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8278,7 +8175,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8364,7 +8261,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8450,7 +8347,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8536,7 +8433,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8627,7 +8524,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8713,7 +8610,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8799,7 +8696,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -8885,7 +8782,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="0" bIns="27432" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -9772,13 +9669,13 @@
         <v>39</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -10107,8 +10004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E8C7D2-1A7F-4BFA-A614-FE10658E33CA}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10155,7 +10052,7 @@
       </c>
       <c r="B3" s="22"/>
       <c r="C3" s="23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>42</v>
@@ -10167,7 +10064,7 @@
       </c>
       <c r="B4" s="22"/>
       <c r="C4" s="23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="22" t="s">
         <v>43</v>
@@ -10178,8 +10075,8 @@
         <v>90</v>
       </c>
       <c r="B5" s="24"/>
-      <c r="C5" s="32" t="b">
-        <v>0</v>
+      <c r="C5" s="23" t="b">
+        <v>1</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>44</v>
@@ -10194,7 +10091,29 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="40962" r:id="rId3" name="Check Box 2">
+            <control shapeId="40963" r:id="rId3" name="Check Box 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>175260</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>457200</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>7620</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="40964" r:id="rId4" name="Check Box 4">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -10205,9 +10124,9 @@
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>464820</xdr:colOff>
+                    <xdr:colOff>472440</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
+                    <xdr:rowOff>15240</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -10216,7 +10135,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="40963" r:id="rId4" name="Check Box 3">
+            <control shapeId="40981" r:id="rId5" name="Check Box 21">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -10227,7 +10146,51 @@
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>464820</xdr:colOff>
+                    <xdr:colOff>472440</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="40982" r:id="rId6" name="Check Box 22">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>7620</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>472440</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>15240</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="40983" r:id="rId7" name="Check Box 23">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>7620</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>472440</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>22860</xdr:rowOff>
                   </to>
@@ -10238,7 +10201,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="40964" r:id="rId5" name="Check Box 4">
+            <control shapeId="40984" r:id="rId8" name="Check Box 24">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -10249,96 +10212,8 @@
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>464820</xdr:colOff>
+                    <xdr:colOff>472440</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="40965" r:id="rId6" name="Check Box 5">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>7620</xdr:colOff>
-                    <xdr:row>1</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>464820</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="40966" r:id="rId7" name="Check Box 6">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>7620</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>464820</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="40967" r:id="rId8" name="Check Box 7">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>7620</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>464820</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>22860</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="40968" r:id="rId9" name="Check Box 8">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>7620</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>2</xdr:col>
-                    <xdr:colOff>464820</xdr:colOff>
-                    <xdr:row>5</xdr:row>
                     <xdr:rowOff>22860</xdr:rowOff>
                   </to>
                 </anchor>
@@ -10357,7 +10232,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10392,7 +10267,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -10400,7 +10275,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -10408,7 +10283,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -10416,7 +10291,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -10424,7 +10299,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -10432,7 +10307,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -10440,7 +10315,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -10448,7 +10323,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -10456,7 +10331,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -10464,7 +10339,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -10472,7 +10347,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -10480,7 +10355,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -10488,7 +10363,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -10496,7 +10371,7 @@
         <v>17</v>
       </c>
       <c r="C16" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -10504,7 +10379,7 @@
         <v>18</v>
       </c>
       <c r="C17" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -10512,7 +10387,7 @@
         <v>19</v>
       </c>
       <c r="C18" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -10520,7 +10395,7 @@
         <v>20</v>
       </c>
       <c r="C19" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -10528,7 +10403,7 @@
         <v>21</v>
       </c>
       <c r="C20" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -10536,7 +10411,7 @@
         <v>22</v>
       </c>
       <c r="C21" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -10544,7 +10419,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -10552,7 +10427,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -10560,100 +10435,100 @@
         <v>25</v>
       </c>
       <c r="C24" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="46" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="46" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="46" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="46" t="s">
         <v>29</v>
       </c>
       <c r="C28" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="46" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="46" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="46" t="s">
         <v>32</v>
       </c>
       <c r="C31" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="46" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="46" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="46" t="s">
         <v>35</v>
       </c>
       <c r="C34" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="46" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="22" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C36" s="22" t="b">
         <v>1</v>
@@ -11447,8 +11322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E5C615-F815-41AB-BEEF-C7C927BFC703}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11507,7 +11382,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F2" t="s">
         <v>124</v>
@@ -11533,7 +11408,7 @@
         <v>137</v>
       </c>
       <c r="D3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="27" t="s">
         <v>61</v>
@@ -11557,9 +11432,11 @@
         <v>138</v>
       </c>
       <c r="D4" t="b">
-        <v>0</v>
-      </c>
-      <c r="E4" s="27"/>
+        <v>1</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>209</v>
+      </c>
       <c r="F4" t="s">
         <v>124</v>
       </c>
@@ -11576,9 +11453,11 @@
         <v>138</v>
       </c>
       <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="27"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>209</v>
+      </c>
       <c r="F5" t="s">
         <v>124</v>
       </c>
@@ -11595,7 +11474,7 @@
         <v>138</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" t="s">
@@ -11617,7 +11496,7 @@
         <v>138</v>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="27"/>
       <c r="F7" t="s">
@@ -11636,7 +11515,7 @@
         <v>139</v>
       </c>
       <c r="D8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="27"/>
       <c r="F8" t="s">
@@ -11655,7 +11534,7 @@
         <v>139</v>
       </c>
       <c r="D9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="27" t="s">
         <v>185</v>
@@ -11671,14 +11550,14 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="38" t="s">
         <v>68</v>
       </c>
       <c r="B10" t="s">
         <v>139</v>
       </c>
       <c r="D10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="27" t="s">
         <v>185</v>
@@ -11691,6 +11570,9 @@
       </c>
       <c r="H10" s="27" t="s">
         <v>194</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -11701,7 +11583,7 @@
         <v>139</v>
       </c>
       <c r="D11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="27" t="s">
         <v>185</v>
@@ -11717,14 +11599,14 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="38" t="s">
         <v>70</v>
       </c>
       <c r="B12" t="s">
         <v>139</v>
       </c>
       <c r="D12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="27" t="s">
         <v>185</v>
@@ -11737,6 +11619,9 @@
       </c>
       <c r="H12" s="27" t="s">
         <v>194</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -11747,7 +11632,7 @@
         <v>139</v>
       </c>
       <c r="D13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="27" t="s">
         <v>185</v>
@@ -11770,7 +11655,7 @@
         <v>140</v>
       </c>
       <c r="D14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="27"/>
       <c r="F14" t="s">
@@ -11789,7 +11674,7 @@
         <v>141</v>
       </c>
       <c r="D15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="27"/>
       <c r="F15" t="s">
@@ -11808,7 +11693,7 @@
         <v>141</v>
       </c>
       <c r="D16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="27"/>
       <c r="F16" t="s">
@@ -11828,9 +11713,6 @@
       </c>
       <c r="C17" s="26" t="s">
         <v>39</v>
-      </c>
-      <c r="D17" t="b">
-        <v>0</v>
       </c>
       <c r="E17" s="27"/>
       <c r="F17" s="38" t="s">
@@ -12198,7 +12080,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12245,7 +12127,7 @@
       <c r="E2" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="45" t="s">
         <v>188</v>
       </c>
     </row>
@@ -12255,7 +12137,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>202</v>
@@ -12263,14 +12145,14 @@
       <c r="E3" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G3" s="47"/>
+      <c r="G3" s="45"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>76</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>202</v>
@@ -12278,14 +12160,14 @@
       <c r="E4" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="47"/>
+      <c r="G4" s="45"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>164</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
         <v>202</v>
@@ -12293,14 +12175,14 @@
       <c r="E5" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G5" s="47"/>
+      <c r="G5" s="45"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>134</v>
       </c>
       <c r="C6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>202</v>
@@ -12308,14 +12190,14 @@
       <c r="E6" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G6" s="47"/>
+      <c r="G6" s="45"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>150</v>
       </c>
       <c r="C7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
         <v>202</v>
@@ -12323,14 +12205,14 @@
       <c r="E7" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G7" s="47"/>
+      <c r="G7" s="45"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>77</v>
       </c>
       <c r="C8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" t="s">
         <v>202</v>
@@ -12338,7 +12220,7 @@
       <c r="E8" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="G8" s="47"/>
+      <c r="G8" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -12519,7 +12401,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C3" sqref="C3:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12576,7 +12458,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E2" s="28" t="s">
         <v>190</v>
@@ -12596,7 +12478,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="27" t="s">
         <v>130</v>
       </c>
       <c r="B3" s="1"/>
@@ -12604,9 +12486,9 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>218</v>
-      </c>
-      <c r="E3" s="43" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" s="28" t="s">
         <v>190</v>
       </c>
       <c r="G3" s="40"/>
@@ -12622,7 +12504,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E4" s="29" t="s">
         <v>207</v>
@@ -12641,34 +12523,40 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
-        <v>221</v>
+      <c r="A5" s="38" t="s">
+        <v>230</v>
       </c>
       <c r="C5" t="b">
         <v>1</v>
       </c>
-      <c r="D5" s="44" t="s">
-        <v>209</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>217</v>
+      <c r="D5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="J5" t="s">
+        <v>231</v>
       </c>
       <c r="L5" s="28" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="38" t="s">
         <v>131</v>
       </c>
       <c r="C6" t="b">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>217</v>
+        <v>216</v>
+      </c>
+      <c r="J6" t="s">
+        <v>232</v>
       </c>
       <c r="L6" s="28" t="s">
         <v>191</v>
@@ -12806,7 +12694,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12844,14 +12732,14 @@
       <c r="G1" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="J1" s="46" t="s">
-        <v>226</v>
+      <c r="J1" s="44" t="s">
+        <v>224</v>
       </c>
       <c r="K1" s="34" t="s">
         <v>168</v>
@@ -12866,7 +12754,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E2" t="s">
         <v>78</v>
@@ -12874,32 +12762,32 @@
       <c r="F2" t="s">
         <v>144</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="H2" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="I2" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="H2" s="45" t="s">
-        <v>223</v>
-      </c>
-      <c r="I2" s="45" t="s">
-        <v>224</v>
-      </c>
       <c r="J2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K2" s="31" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="27" t="s">
         <v>196</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E3" t="s">
         <v>79</v>
@@ -12908,16 +12796,16 @@
         <v>144</v>
       </c>
       <c r="G3" t="s">
-        <v>222</v>
-      </c>
-      <c r="H3" s="45" t="s">
+        <v>220</v>
+      </c>
+      <c r="H3" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="I3" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="J3" t="s">
         <v>225</v>
-      </c>
-      <c r="J3" t="s">
-        <v>227</v>
       </c>
       <c r="K3" s="31" t="s">
         <v>148</v>
@@ -12928,35 +12816,41 @@
         <v>197</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>209</v>
       </c>
       <c r="E4" t="s">
         <v>78</v>
       </c>
       <c r="G4" s="38"/>
-      <c r="H4" s="45" t="s">
-        <v>223</v>
-      </c>
-      <c r="I4" s="45" t="s">
-        <v>224</v>
+      <c r="H4" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="I4" s="43" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="27" t="s">
         <v>198</v>
       </c>
       <c r="C5" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>209</v>
       </c>
       <c r="E5" t="s">
         <v>79</v>
       </c>
       <c r="G5" s="38"/>
-      <c r="H5" s="45" t="s">
+      <c r="H5" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="I5" s="43" t="s">
         <v>223</v>
-      </c>
-      <c r="I5" s="45" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -13204,7 +13098,7 @@
         <v>159</v>
       </c>
       <c r="C3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D3" s="35" t="s">
         <v>181</v>
@@ -13229,7 +13123,7 @@
         <v>161</v>
       </c>
       <c r="C5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D5" s="35" t="s">
         <v>183</v>
@@ -13252,12 +13146,12 @@
         <v>153</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D8" s="35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>